<commit_message>
update phandango files, remove KL99, rename K-type designation of K96 to K54_K96
</commit_message>
<xml_diff>
--- a/Database_change_history.xlsx
+++ b/Database_change_history.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccgl/UiO Dropbox/Rebecca Gladstone/Oslo/Ecoli/analyses/K-antigen/alleles_rename/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccgl/UiO Dropbox/Rebecca Gladstone/Oslo/Ecoli/analyses/K-revisions/EC-K-typing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18086FC3-6172-A84C-BCBE-641F01F92F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1F037B-8EDC-AA4B-A280-6B3529AF89A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="660" windowWidth="29220" windowHeight="28140" xr2:uid="{8D4199F1-83C8-C04F-B8D3-FBA17DA55378}"/>
+    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" xr2:uid="{8D4199F1-83C8-C04F-B8D3-FBA17DA55378}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Action</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t xml:space="preserve">KL14 is assigned to isolates that are confirmed to phenotype as K24 (MG739439) or K6 (ERZ24125990), the genetic basic for this difference is not known. </t>
+  </si>
+  <si>
+    <t>KL99</t>
+  </si>
+  <si>
+    <t>Frequent mistyping of KL13 as KL99. KL99 differs from KL13 and KL34 by a duplication of  group 154.</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,7 +190,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,29 +526,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798FA74E-E96E-9F49-A7B5-E889396D1818}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="20.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.83203125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -743,8 +746,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45901</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>

</xml_diff>